<commit_message>
Adding refactoring to the main and graph to accept inverted types of graphs and unpack data from bidirectional a-star
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -12,6 +12,8 @@
     <sheet name="IDA" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="SMA" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="RTAA (lookahead=25, move_limit=" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="RTAA (L=25,M=3)" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="RTAA (L=25, M=3)" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,12 +449,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Metric</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
@@ -463,7 +465,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001676669999142177</v>
+        <v>0.0002895420002460014</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +475,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0001639169995542034</v>
+        <v>0.0001696250001259614</v>
       </c>
     </row>
     <row r="4">
@@ -483,7 +485,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>199</v>
+        <v>3404.2</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +495,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>199</v>
+        <v>4011.8</v>
       </c>
     </row>
     <row r="6">
@@ -503,7 +505,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.01345062255859375</v>
+        <v>0.00292205810546875</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +515,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.01336517333984375</v>
+        <v>0.00286712646484375</v>
       </c>
     </row>
     <row r="8">
@@ -523,7 +525,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.0112152099609375</v>
+        <v>0.006529808044433594</v>
       </c>
     </row>
     <row r="9">
@@ -533,7 +535,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.0112152099609375</v>
+        <v>0.006529808044433594</v>
       </c>
     </row>
     <row r="10">
@@ -543,7 +545,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>5.425000017567072e-05</v>
+        <v>4.350000017439015e-05</v>
       </c>
     </row>
     <row r="11">
@@ -553,7 +555,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>5.429199973150389e-05</v>
+        <v>4.154199996264651e-05</v>
       </c>
     </row>
     <row r="12">
@@ -563,7 +565,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>5.035839994889102e-05</v>
+        <v>4.760915995575488e-05</v>
       </c>
     </row>
     <row r="13">
@@ -573,7 +575,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.858770016653579e-05</v>
+        <v>2.677832000699709e-05</v>
       </c>
     </row>
     <row r="14">
@@ -583,7 +585,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -612,12 +614,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Metric</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
@@ -628,7 +630,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001584159999765689</v>
+        <v>0.0001489170008426299</v>
       </c>
     </row>
     <row r="3">
@@ -638,7 +640,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.004422250000061467</v>
+        <v>0.0009407919988007052</v>
       </c>
     </row>
     <row r="4">
@@ -648,7 +650,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>199</v>
+        <v>3404.2</v>
       </c>
     </row>
     <row r="5">
@@ -658,7 +660,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>199</v>
+        <v>3404.2</v>
       </c>
     </row>
     <row r="6">
@@ -668,7 +670,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.02333831787109375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="7">
@@ -678,7 +680,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.01534271240234375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="8">
@@ -688,7 +690,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>1.978477478027344</v>
+        <v>0.07830810546875</v>
       </c>
     </row>
     <row r="9">
@@ -698,7 +700,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1.959867858886719</v>
+        <v>0.07816162109374999</v>
       </c>
     </row>
     <row r="10">
@@ -708,7 +710,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.0003252489996157237</v>
+        <v>0.000202334000277915</v>
       </c>
     </row>
     <row r="11">
@@ -718,7 +720,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0006816240002081031</v>
+        <v>0.0002507919998606667</v>
       </c>
     </row>
     <row r="12">
@@ -728,7 +730,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2.486240000507678e-05</v>
+        <v>4.610631001924048e-05</v>
       </c>
     </row>
     <row r="13">
@@ -738,7 +740,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1.949999996213592e-05</v>
+        <v>2.092377006192692e-05</v>
       </c>
     </row>
     <row r="14">
@@ -748,7 +750,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -777,12 +779,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Metric</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
@@ -793,7 +795,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001360419992124662</v>
+        <v>0.0003603750010370277</v>
       </c>
     </row>
     <row r="3">
@@ -803,7 +805,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.001159166999968875</v>
+        <v>0.06191437499910535</v>
       </c>
     </row>
     <row r="4">
@@ -813,7 +815,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>199</v>
+        <v>3404.2</v>
       </c>
     </row>
     <row r="5">
@@ -823,7 +825,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>199</v>
+        <v>3404.2</v>
       </c>
     </row>
     <row r="6">
@@ -833,7 +835,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.01334381103515625</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="7">
@@ -843,7 +845,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.01334381103515625</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="8">
@@ -853,7 +855,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.00339508056640625</v>
+        <v>0.00331878662109375</v>
       </c>
     </row>
     <row r="9">
@@ -863,7 +865,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.00325469970703125</v>
+        <v>0.00316009521484375</v>
       </c>
     </row>
     <row r="10">
@@ -873,7 +875,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>5.34999999217689e-05</v>
+        <v>4.237500070303213e-05</v>
       </c>
     </row>
     <row r="11">
@@ -883,7 +885,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0009795000005397014</v>
+        <v>0.04104479200032074</v>
       </c>
     </row>
     <row r="12">
@@ -893,7 +895,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.0009750540000823093</v>
+        <v>0.003269873690023815</v>
       </c>
     </row>
     <row r="13">
@@ -903,7 +905,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.989600010958384e-05</v>
+        <v>3.284329002781306e-05</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +915,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -942,12 +944,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Metric</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
@@ -958,7 +960,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001581669994266122</v>
+        <v>0.0003745829999388661</v>
       </c>
     </row>
     <row r="3">
@@ -968,7 +970,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0001078750001397566</v>
+        <v>6.912499884492718e-05</v>
       </c>
     </row>
     <row r="4">
@@ -978,7 +980,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>199</v>
+        <v>3404.2</v>
       </c>
     </row>
     <row r="5">
@@ -988,7 +990,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>199</v>
+        <v>6223.7</v>
       </c>
     </row>
     <row r="6">
@@ -998,7 +1000,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.01334381103515625</v>
+        <v>0.00292205810546875</v>
       </c>
     </row>
     <row r="7">
@@ -1008,7 +1010,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.01334381103515625</v>
+        <v>0.00290374755859375</v>
       </c>
     </row>
     <row r="8">
@@ -1018,7 +1020,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.01338958740234375</v>
+        <v>0.00208282470703125</v>
       </c>
     </row>
     <row r="9">
@@ -1028,7 +1030,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.01338958740234375</v>
+        <v>0.00208282470703125</v>
       </c>
     </row>
     <row r="10">
@@ -1038,7 +1040,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>5.316600072546862e-05</v>
+        <v>4.466700011107605e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1048,7 +1050,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>8.954199984145816e-05</v>
+        <v>5.137500011187512e-05</v>
       </c>
     </row>
     <row r="12">
@@ -1058,7 +1060,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>8.777490011198097e-05</v>
+        <v>4.544505989542813e-05</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1070,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>5.07915000525827e-05</v>
+        <v>3.024249006557511e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1078,7 +1080,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1249,4 +1251,334 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="26" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Métrica</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>A* Time (s)</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.0001922079991345527</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Time (s)</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.0002124579987139441</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>A* Cost</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>3404.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Cost</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4781.1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>A* Peak Memory (MiB)</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0.00290679931640625</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>A* Avg Memory (MiB)</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.00286407470703125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Peak Memory (MiB)</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.00658416748046875</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Avg Memory (MiB)</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>0.00658416748046875</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>A* Recalc Time (s)</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>4.41249994764803e-05</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Recalc Time (s)</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>0.0001134170015575364</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Bulk Avg Time (s)</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>6.257919994823169e-05</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>A* Bulk Avg Time (s)</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>2.519559984648367e-05</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Bulk Modifications Count</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="26" customWidth="1" min="1" max="1"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>A* Time (s)</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.0001582920012879185</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Time (s)</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.0002144169993698597</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>A* Cost</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>3404.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Cost</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4781.1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>A* Peak Memory (MiB)</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0.00290679931640625</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>A* Avg Memory (MiB)</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.00286407470703125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Peak Memory (MiB)</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.00658416748046875</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Avg Memory (MiB)</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>0.00658416748046875</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>A* Recalc Time (s)</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>4.400000034365803e-05</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Recalc Time (s)</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>0.0001148749997810228</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>RTAA* Bulk Avg Time (s)</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>8.915325994166778e-05</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>A* Bulk Avg Time (s)</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>3.22303500615817e-05</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Bulk Modifications Count</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding metrics into Graphs
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0003272500034654513</v>
+        <v>0.0001732079836074263</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0003042500029550865</v>
+        <v>0.0001627909950911999</v>
       </c>
     </row>
     <row r="4">
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.962499951943755e-05</v>
+        <v>4.66250057797879e-05</v>
       </c>
     </row>
     <row r="11">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>4.666599852498621e-05</v>
+        <v>4.233297659084201e-05</v>
       </c>
     </row>
     <row r="12">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>4.528214121819474e-05</v>
+        <v>2.058133890386671e-05</v>
       </c>
     </row>
     <row r="13">
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>3.053957960219123e-05</v>
+        <v>2.205587952630594e-05</v>
       </c>
     </row>
     <row r="14">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001537909993203357</v>
+        <v>0.0001530419976916164</v>
       </c>
     </row>
     <row r="3">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.001008917010040022</v>
+        <v>0.001183999993372709</v>
       </c>
     </row>
     <row r="4">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.0002349989954382181</v>
+        <v>0.0002400420198682696</v>
       </c>
     </row>
     <row r="11">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0002502090064808726</v>
+        <v>0.0007048329862300307</v>
       </c>
     </row>
     <row r="12">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2.769997052382678e-05</v>
+        <v>2.595293044578284e-05</v>
       </c>
     </row>
     <row r="13">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>9.37132048420608e-06</v>
+        <v>1.868125109467655e-05</v>
       </c>
     </row>
     <row r="14">
@@ -773,7 +773,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="26" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0002852500037988648</v>
+        <v>0.0002098749973811209</v>
       </c>
     </row>
     <row r="3">
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0468188340018969</v>
+        <v>0.04566537501523271</v>
       </c>
     </row>
     <row r="4">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.00319671630859375</v>
+        <v>0.00330352783203125</v>
       </c>
     </row>
     <row r="9">
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.00312347412109375</v>
+        <v>0.00314483642578125</v>
       </c>
     </row>
     <row r="10">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.562499816529453e-05</v>
+        <v>4.50420193374157e-05</v>
       </c>
     </row>
     <row r="11">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.04172091699729208</v>
+        <v>0.04108999998425134</v>
       </c>
     </row>
     <row r="12">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.002589604630193207</v>
+        <v>0.1462675570798456</v>
       </c>
     </row>
     <row r="13">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2.527077987906523e-05</v>
+        <v>4.112749971682205e-05</v>
       </c>
     </row>
     <row r="14">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001740410079946741</v>
+        <v>0.000164999975822866</v>
       </c>
     </row>
     <row r="3">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.870900011155754e-05</v>
+        <v>4.358400474302471e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>6.150000263005495e-05</v>
+        <v>5.779098137281835e-05</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>7.011333989794366e-05</v>
+        <v>6.073289026971906e-05</v>
       </c>
     </row>
     <row r="13">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>5.080628034193069e-05</v>
+        <v>4.274330916814506e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0003580420016078278</v>
+        <v>0.0002497080131433904</v>
       </c>
     </row>
     <row r="3">
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0003091659891651943</v>
+        <v>0.0002369160065427423</v>
       </c>
     </row>
     <row r="4">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>9.258300997316837e-05</v>
+        <v>9.741701069287956e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0002444169949740171</v>
+        <v>0.0002357499906793237</v>
       </c>
     </row>
     <row r="12">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.000148137569631217</v>
+        <v>0.0001182457999675535</v>
       </c>
     </row>
     <row r="13">
@@ -1565,7 +1565,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>5.020252967369742e-05</v>
+        <v>4.383333958685398e-05</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
IDA* memory usage and speed updates. Path is no longer stored in full on every iteration
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -443,7 +443,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="36" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001732079836074263</v>
+        <v>0.0006103999985498376</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0001627909950911999</v>
+        <v>0.0006560000038007274</v>
       </c>
     </row>
     <row r="4">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.00284576416015625</v>
+        <v>0.00292205810546875</v>
       </c>
     </row>
     <row r="7">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.00279083251953125</v>
+        <v>0.00286712646484375</v>
       </c>
     </row>
     <row r="8">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.006537437438964844</v>
+        <v>0.006529808044433594</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.006537437438964844</v>
+        <v>0.006529808044433594</v>
       </c>
     </row>
     <row r="10">
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.66250057797879e-05</v>
+        <v>8.159999561030418e-05</v>
       </c>
     </row>
     <row r="11">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>4.233297659084201e-05</v>
+        <v>8.369999704882503e-05</v>
       </c>
     </row>
     <row r="12">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2.058133890386671e-05</v>
+        <v>7.849099951272365e-05</v>
       </c>
     </row>
     <row r="13">
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2.205587952630594e-05</v>
+        <v>6.802499992772937e-05</v>
       </c>
     </row>
     <row r="14">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001530419976916164</v>
+        <v>0.0003914999979315326</v>
       </c>
     </row>
     <row r="3">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.001183999993372709</v>
+        <v>0.002471799998602364</v>
       </c>
     </row>
     <row r="4">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.002777099609375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="7">
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.002777099609375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="8">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.07778167724609375</v>
+        <v>0.07830810546875</v>
       </c>
     </row>
     <row r="9">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.07764892578125</v>
+        <v>0.07811584472656249</v>
       </c>
     </row>
     <row r="10">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.0002400420198682696</v>
+        <v>0.000622500003373716</v>
       </c>
     </row>
     <row r="11">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0007048329862300307</v>
+        <v>0.0008314000006066635</v>
       </c>
     </row>
     <row r="12">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2.595293044578284e-05</v>
+        <v>5.738300053053536e-05</v>
       </c>
     </row>
     <row r="13">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1.868125109467655e-05</v>
+        <v>2.851799989002757e-05</v>
       </c>
     </row>
     <row r="14">
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0002098749973811209</v>
+        <v>0.0003122999987681396</v>
       </c>
     </row>
     <row r="3">
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.04566537501523271</v>
+        <v>0.003447600000072271</v>
       </c>
     </row>
     <row r="4">
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.002777099609375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="7">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.002777099609375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="8">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.00330352783203125</v>
+        <v>0.0027618408203125</v>
       </c>
     </row>
     <row r="9">
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.00314483642578125</v>
+        <v>0.0026763916015625</v>
       </c>
     </row>
     <row r="10">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.50420193374157e-05</v>
+        <v>0.0001033000007737428</v>
       </c>
     </row>
     <row r="11">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.04108999998425134</v>
+        <v>0.003874099995300639</v>
       </c>
     </row>
     <row r="12">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.1462675570798456</v>
+        <v>0.001430455000154325</v>
       </c>
     </row>
     <row r="13">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.112749971682205e-05</v>
+        <v>8.190399981685914e-05</v>
       </c>
     </row>
     <row r="14">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.000164999975822866</v>
+        <v>0.000745400000596419</v>
       </c>
     </row>
     <row r="3">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>6.937500438652933e-05</v>
+        <v>0.0002872999975807033</v>
       </c>
     </row>
     <row r="4">
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.0028228759765625</v>
+        <v>0.002899169921875</v>
       </c>
     </row>
     <row r="7">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.00281829833984375</v>
+        <v>0.00289459228515625</v>
       </c>
     </row>
     <row r="8">
@@ -1020,7 +1020,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.00264739990234375</v>
+        <v>0.00261688232421875</v>
       </c>
     </row>
     <row r="9">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.00264739990234375</v>
+        <v>0.00261688232421875</v>
       </c>
     </row>
     <row r="10">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.358400474302471e-05</v>
+        <v>8.789999992586672e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>5.779098137281835e-05</v>
+        <v>0.0001325999983237125</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>6.073289026971906e-05</v>
+        <v>0.0001251799998863135</v>
       </c>
     </row>
     <row r="13">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.274330916814506e-05</v>
+        <v>8.085900022706482e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0002497080131433904</v>
+        <v>0.001102899994293693</v>
       </c>
     </row>
     <row r="3">
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0002369160065427423</v>
+        <v>0.001140100001066457</v>
       </c>
     </row>
     <row r="4">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.00283050537109375</v>
+        <v>0.00290679931640625</v>
       </c>
     </row>
     <row r="7">
@@ -1505,7 +1505,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.00278778076171875</v>
+        <v>0.00286407470703125</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1515,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.0066070556640625</v>
+        <v>0.00658416748046875</v>
       </c>
     </row>
     <row r="9">
@@ -1525,7 +1525,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.0066070556640625</v>
+        <v>0.00658416748046875</v>
       </c>
     </row>
     <row r="10">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>9.741701069287956e-05</v>
+        <v>0.0002367999986745417</v>
       </c>
     </row>
     <row r="11">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0002357499906793237</v>
+        <v>0.0005340999996406026</v>
       </c>
     </row>
     <row r="12">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.0001182457999675535</v>
+        <v>0.0003921499994612532</v>
       </c>
     </row>
     <row r="13">
@@ -1565,7 +1565,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.383333958685398e-05</v>
+        <v>0.0001180289998592343</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
Adding new functionality to show graph
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001732079836074263</v>
+        <v>0.0001963750000868458</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0001627909950911999</v>
+        <v>0.0002029580009548226</v>
       </c>
     </row>
     <row r="4">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>3404.2</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="5">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>4011.8</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="6">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.00284576416015625</v>
+        <v>0.00315093994140625</v>
       </c>
     </row>
     <row r="7">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.00279083251953125</v>
+        <v>0.00309600830078125</v>
       </c>
     </row>
     <row r="8">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.006537437438964844</v>
+        <v>0.0084991455078125</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.006537437438964844</v>
+        <v>0.0084991455078125</v>
       </c>
     </row>
     <row r="10">
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.66250057797879e-05</v>
+        <v>4.362500112620182e-05</v>
       </c>
     </row>
     <row r="11">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>4.233297659084201e-05</v>
+        <v>6.170900087454356e-05</v>
       </c>
     </row>
     <row r="12">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2.058133890386671e-05</v>
+        <v>2.179581254040386e-05</v>
       </c>
     </row>
     <row r="13">
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2.205587952630594e-05</v>
+        <v>4.326136256622703e-05</v>
       </c>
     </row>
     <row r="14">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001530419976916164</v>
+        <v>0.000353749999703723</v>
       </c>
     </row>
     <row r="3">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.001183999993372709</v>
+        <v>0.001694665999821154</v>
       </c>
     </row>
     <row r="4">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>3404.2</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="5">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>3404.2</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.002777099609375</v>
+        <v>0.003082275390625</v>
       </c>
     </row>
     <row r="7">
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.002777099609375</v>
+        <v>0.003082275390625</v>
       </c>
     </row>
     <row r="8">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.07778167724609375</v>
+        <v>0.07830810546875</v>
       </c>
     </row>
     <row r="9">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.07764892578125</v>
+        <v>0.07805328369140625</v>
       </c>
     </row>
     <row r="10">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.0002400420198682696</v>
+        <v>0.0002877090009860694</v>
       </c>
     </row>
     <row r="11">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0007048329862300307</v>
+        <v>0.0008845000011206139</v>
       </c>
     </row>
     <row r="12">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2.595293044578284e-05</v>
+        <v>0.0001083754750425214</v>
       </c>
     </row>
     <row r="13">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1.868125109467655e-05</v>
+        <v>4.761206259900064e-05</v>
       </c>
     </row>
     <row r="14">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +773,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="26" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0002098749973811209</v>
+        <v>0.0001899170001706807</v>
       </c>
     </row>
     <row r="3">
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.04566537501523271</v>
+        <v>0.009287000000767875</v>
       </c>
     </row>
     <row r="4">
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>3404.2</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="5">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>3404.2</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="6">
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.002777099609375</v>
+        <v>0.003082275390625</v>
       </c>
     </row>
     <row r="7">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.002777099609375</v>
+        <v>0.003082275390625</v>
       </c>
     </row>
     <row r="8">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.00330352783203125</v>
+        <v>0.00305938720703125</v>
       </c>
     </row>
     <row r="9">
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.00314483642578125</v>
+        <v>0.00300445556640625</v>
       </c>
     </row>
     <row r="10">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.50420193374157e-05</v>
+        <v>6.512499930977356e-05</v>
       </c>
     </row>
     <row r="11">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.04108999998425134</v>
+        <v>0.005360707998988801</v>
       </c>
     </row>
     <row r="12">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.1462675570798456</v>
+        <v>0.008276711987468844</v>
       </c>
     </row>
     <row r="13">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.112749971682205e-05</v>
+        <v>4.337861246312968e-05</v>
       </c>
     </row>
     <row r="14">
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.000164999975822866</v>
+        <v>0.0001857920015027048</v>
       </c>
     </row>
     <row r="3">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>6.937500438652933e-05</v>
+        <v>6.320799911918584e-05</v>
       </c>
     </row>
     <row r="4">
@@ -980,7 +980,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>3404.2</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="5">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>3404.2</v>
+        <v>6729.199999999999</v>
       </c>
     </row>
     <row r="6">
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.0028228759765625</v>
+        <v>0.00315093994140625</v>
       </c>
     </row>
     <row r="7">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.00281829833984375</v>
+        <v>0.00313262939453125</v>
       </c>
     </row>
     <row r="8">
@@ -1020,7 +1020,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.00264739990234375</v>
+        <v>0.00220489501953125</v>
       </c>
     </row>
     <row r="9">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.00264739990234375</v>
+        <v>0.00220489501953125</v>
       </c>
     </row>
     <row r="10">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.358400474302471e-05</v>
+        <v>4.333299875725061e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>5.779098137281835e-05</v>
+        <v>3.950000063923653e-05</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>6.073289026971906e-05</v>
+        <v>0.0001048161124572289</v>
       </c>
     </row>
     <row r="13">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.274330916814506e-05</v>
+        <v>6.615983757001232e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1433,7 +1433,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="26" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0002497080131433904</v>
+        <v>0.0004321249998611165</v>
       </c>
     </row>
     <row r="3">
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0002369160065427423</v>
+        <v>0.0004928750004182803</v>
       </c>
     </row>
     <row r="4">
@@ -1475,7 +1475,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>3404.2</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="5">
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>4781.1</v>
+        <v>5431.7</v>
       </c>
     </row>
     <row r="6">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.00283050537109375</v>
+        <v>0.00313568115234375</v>
       </c>
     </row>
     <row r="7">
@@ -1505,7 +1505,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.00278778076171875</v>
+        <v>0.00309295654296875</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1515,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.0066070556640625</v>
+        <v>0.00685882568359375</v>
       </c>
     </row>
     <row r="9">
@@ -1525,7 +1525,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.0066070556640625</v>
+        <v>0.00685882568359375</v>
       </c>
     </row>
     <row r="10">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>9.741701069287956e-05</v>
+        <v>4.429200089361984e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0002357499906793237</v>
+        <v>0.0001279580010304926</v>
       </c>
     </row>
     <row r="12">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.0001182457999675535</v>
+        <v>0.0001367577998962588</v>
       </c>
     </row>
     <row r="13">
@@ -1565,7 +1565,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.383333958685398e-05</v>
+        <v>4.306251253183291e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalize part to add plots
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -14,6 +14,7 @@
     <sheet name="RTAA (lookahead=25, move_limit=" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="RTAA (L=25,M=3)" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="RTAA (L=25, M=3)" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="A" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -465,7 +466,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001317080004810123</v>
+        <v>0.0001506669996160781</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +476,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0001403749993187375</v>
+        <v>0.0001620410002942663</v>
       </c>
     </row>
     <row r="4">
@@ -485,7 +486,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1600.8</v>
+        <v>2677.5408</v>
       </c>
     </row>
     <row r="5">
@@ -495,7 +496,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1600.8</v>
+        <v>2790.3315</v>
       </c>
     </row>
     <row r="6">
@@ -505,7 +506,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.00240325927734375</v>
+        <v>0.00287628173828125</v>
       </c>
     </row>
     <row r="7">
@@ -515,7 +516,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.00233612060546875</v>
+        <v>0.00285797119140625</v>
       </c>
     </row>
     <row r="8">
@@ -525,7 +526,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.005446434020996094</v>
+        <v>0.0084381103515625</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +536,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.005446434020996094</v>
+        <v>0.0084381103515625</v>
       </c>
     </row>
     <row r="10">
@@ -545,7 +546,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>2.529099947423674e-05</v>
+        <v>4.329200055508409e-05</v>
       </c>
     </row>
     <row r="11">
@@ -555,7 +556,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3.054199987673201e-05</v>
+        <v>5.59170002816245e-05</v>
       </c>
     </row>
     <row r="12">
@@ -565,7 +566,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2.741250009421492e-05</v>
+        <v>4.169159983575809e-05</v>
       </c>
     </row>
     <row r="13">
@@ -575,7 +576,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2.936670007329667e-05</v>
+        <v>4.960019978170749e-05</v>
       </c>
     </row>
     <row r="14">
@@ -585,7 +586,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +631,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.00027179199969396</v>
+        <v>0.0001537499992991798</v>
       </c>
     </row>
     <row r="3">
@@ -640,7 +641,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0006209580005815951</v>
+        <v>0.001023999999233638</v>
       </c>
     </row>
     <row r="4">
@@ -650,7 +651,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1600.8</v>
+        <v>2677.5408</v>
       </c>
     </row>
     <row r="5">
@@ -660,7 +661,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1600.8</v>
+        <v>2677.5408</v>
       </c>
     </row>
     <row r="6">
@@ -670,7 +671,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.0023193359375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="7">
@@ -680,7 +681,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.0023193359375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="8">
@@ -690,7 +691,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.07711029052734375</v>
+        <v>0.07726287841796875</v>
       </c>
     </row>
     <row r="9">
@@ -700,7 +701,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.07694091796874999</v>
+        <v>0.07698516845703125</v>
       </c>
     </row>
     <row r="10">
@@ -710,7 +711,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.00043366800127842</v>
+        <v>0.0002467909998813411</v>
       </c>
     </row>
     <row r="11">
@@ -720,7 +721,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0009517090002191253</v>
+        <v>0.0008286670017696451</v>
       </c>
     </row>
     <row r="12">
@@ -730,7 +731,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>3.135830029350472e-05</v>
+        <v>4.184159988653846e-05</v>
       </c>
     </row>
     <row r="13">
@@ -740,7 +741,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2.391250000073342e-05</v>
+        <v>4.28502000431763e-05</v>
       </c>
     </row>
     <row r="14">
@@ -750,7 +751,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +774,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="26" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -795,7 +796,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0003760420004255138</v>
+        <v>0.00025558400011505</v>
       </c>
     </row>
     <row r="3">
@@ -805,7 +806,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0009264170003007166</v>
+        <v>0.01366037499974482</v>
       </c>
     </row>
     <row r="4">
@@ -815,7 +816,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1600.8</v>
+        <v>2677.5408</v>
       </c>
     </row>
     <row r="5">
@@ -825,7 +826,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1600.8</v>
+        <v>2677.5408</v>
       </c>
     </row>
     <row r="6">
@@ -835,7 +836,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.0023193359375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="7">
@@ -845,7 +846,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.0023193359375</v>
+        <v>0.0028533935546875</v>
       </c>
     </row>
     <row r="8">
@@ -855,7 +856,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.002044677734375</v>
+        <v>0.0026397705078125</v>
       </c>
     </row>
     <row r="9">
@@ -865,7 +866,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.00198974609375</v>
+        <v>0.0025848388671875</v>
       </c>
     </row>
     <row r="10">
@@ -875,7 +876,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3.262499922129791e-05</v>
+        <v>4.600000102072954e-05</v>
       </c>
     </row>
     <row r="11">
@@ -885,7 +886,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0003493749991321238</v>
+        <v>0.01290912500007835</v>
       </c>
     </row>
     <row r="12">
@@ -895,7 +896,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.00069495400039159</v>
+        <v>0.01184026660012023</v>
       </c>
     </row>
     <row r="13">
@@ -905,7 +906,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>3.257919997849968e-05</v>
+        <v>4.02916000894038e-05</v>
       </c>
     </row>
     <row r="14">
@@ -915,7 +916,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -960,7 +961,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001792500006558839</v>
+        <v>0.0001817499996832339</v>
       </c>
     </row>
     <row r="3">
@@ -970,7 +971,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>6.6917000367539e-05</v>
+        <v>7.399999958579428e-05</v>
       </c>
     </row>
     <row r="4">
@@ -980,7 +981,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1600.8</v>
+        <v>2677.5408</v>
       </c>
     </row>
     <row r="5">
@@ -990,7 +991,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1600.8</v>
+        <v>2677.5408</v>
       </c>
     </row>
     <row r="6">
@@ -1000,7 +1001,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.0023193359375</v>
+        <v>0.00287628173828125</v>
       </c>
     </row>
     <row r="7">
@@ -1010,7 +1011,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.0023193359375</v>
+        <v>0.00285797119140625</v>
       </c>
     </row>
     <row r="8">
@@ -1040,7 +1041,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>2.462500015099067e-05</v>
+        <v>4.366699977254029e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1050,7 +1051,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>4.816600085177924e-05</v>
+        <v>5.908300045120995e-05</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1061,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.0001177043001007405</v>
+        <v>5.871680041309446e-05</v>
       </c>
     </row>
     <row r="13">
@@ -1070,7 +1071,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.621259959094459e-05</v>
+        <v>3.793340038100723e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1080,7 +1081,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1455,7 +1456,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001410839995514834</v>
+        <v>0.0001637500008655479</v>
       </c>
     </row>
     <row r="3">
@@ -1465,7 +1466,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0001639170004636981</v>
+        <v>0.000217417000385467</v>
       </c>
     </row>
     <row r="4">
@@ -1475,7 +1476,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1600.8</v>
+        <v>2677.5408</v>
       </c>
     </row>
     <row r="5">
@@ -1485,7 +1486,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1600.8</v>
+        <v>3484.7703</v>
       </c>
     </row>
     <row r="6">
@@ -1495,7 +1496,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.0023193359375</v>
+        <v>0.00290679931640625</v>
       </c>
     </row>
     <row r="7">
@@ -1505,7 +1506,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.0023193359375</v>
+        <v>0.00286407470703125</v>
       </c>
     </row>
     <row r="8">
@@ -1515,7 +1516,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.00458526611328125</v>
+        <v>0.00658416748046875</v>
       </c>
     </row>
     <row r="9">
@@ -1525,7 +1526,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.00458526611328125</v>
+        <v>0.00658416748046875</v>
       </c>
     </row>
     <row r="10">
@@ -1535,7 +1536,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>2.524999945308082e-05</v>
+        <v>4.354100019554608e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1545,7 +1546,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>6.000000030326191e-05</v>
+        <v>0.0001148749997810228</v>
       </c>
     </row>
     <row r="12">
@@ -1555,7 +1556,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>6.486240035883384e-05</v>
+        <v>0.0001135832004365511</v>
       </c>
     </row>
     <row r="13">
@@ -1565,7 +1566,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2.752529999270337e-05</v>
+        <v>3.740840002137702e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1575,7 +1576,62 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>2677.5408</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Path length</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding also original view of graph
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -443,7 +443,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="36" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0006103999985498376</v>
+        <v>0.0001949170000443701</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0006560000038007274</v>
+        <v>0.0001602500014996622</v>
       </c>
     </row>
     <row r="4">
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>8.159999561030418e-05</v>
+        <v>4.370800161268562e-05</v>
       </c>
     </row>
     <row r="11">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>8.369999704882503e-05</v>
+        <v>4.137499854550697e-05</v>
       </c>
     </row>
     <row r="12">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>7.849099951272365e-05</v>
+        <v>4.085913016751874e-05</v>
       </c>
     </row>
     <row r="13">
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>6.802499992772937e-05</v>
+        <v>2.335323981242254e-05</v>
       </c>
     </row>
     <row r="14">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0003914999979315326</v>
+        <v>0.0001353750012640376</v>
       </c>
     </row>
     <row r="3">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.002471799998602364</v>
+        <v>0.0009342499979538843</v>
       </c>
     </row>
     <row r="4">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.07811584472656249</v>
+        <v>0.07813873291015624</v>
       </c>
     </row>
     <row r="10">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.000622500003373716</v>
+        <v>0.0002485410041117575</v>
       </c>
     </row>
     <row r="11">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0008314000006066635</v>
+        <v>0.0008862069989845622</v>
       </c>
     </row>
     <row r="12">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>5.738300053053536e-05</v>
+        <v>2.574538015323924e-05</v>
       </c>
     </row>
     <row r="13">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2.851799989002757e-05</v>
+        <v>1.349297006527195e-05</v>
       </c>
     </row>
     <row r="14">
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0003122999987681396</v>
+        <v>0.0001340829985565506</v>
       </c>
     </row>
     <row r="3">
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.003447600000072271</v>
+        <v>0.002364125000895001</v>
       </c>
     </row>
     <row r="4">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.0001033000007737428</v>
+        <v>4.945800174027681e-05</v>
       </c>
     </row>
     <row r="11">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.003874099995300639</v>
+        <v>0.002018958002736326</v>
       </c>
     </row>
     <row r="12">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.001430455000154325</v>
+        <v>0.003498007900052471</v>
       </c>
     </row>
     <row r="13">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>8.190399981685914e-05</v>
+        <v>6.50303599104518e-05</v>
       </c>
     </row>
     <row r="14">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.000745400000596419</v>
+        <v>0.0001991669996641576</v>
       </c>
     </row>
     <row r="3">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0002872999975807033</v>
+        <v>7.337499846471474e-05</v>
       </c>
     </row>
     <row r="4">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>8.789999992586672e-05</v>
+        <v>4.312499731895514e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0001325999983237125</v>
+        <v>5.63749999855645e-05</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.0001251799998863135</v>
+        <v>5.652378982631489e-05</v>
       </c>
     </row>
     <row r="13">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>8.085900022706482e-05</v>
+        <v>3.881909018673468e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.001102899994293693</v>
+        <v>0.0002321669999219012</v>
       </c>
     </row>
     <row r="3">
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.001140100001066457</v>
+        <v>0.00022641699979431</v>
       </c>
     </row>
     <row r="4">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.0002367999986745417</v>
+        <v>4.275000173947774e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0005340999996406026</v>
+        <v>0.0001147090006270446</v>
       </c>
     </row>
     <row r="12">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.0003921499994612532</v>
+        <v>0.0003925650500241318</v>
       </c>
     </row>
     <row r="13">
@@ -1565,7 +1565,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0.0001180289998592343</v>
+        <v>6.946291970962193e-05</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
Updating Graphs code to print in different ways.
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001949170000443701</v>
+        <v>0.000150040999869816</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0001602500014996622</v>
+        <v>0.0001546659987070598</v>
       </c>
     </row>
     <row r="4">
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.370800161268562e-05</v>
+        <v>4.179200186626986e-05</v>
       </c>
     </row>
     <row r="11">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>4.137499854550697e-05</v>
+        <v>4.037500184495002e-05</v>
       </c>
     </row>
     <row r="12">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>4.085913016751874e-05</v>
+        <v>3.634379951108712e-05</v>
       </c>
     </row>
     <row r="13">
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2.335323981242254e-05</v>
+        <v>2.771832056168933e-05</v>
       </c>
     </row>
     <row r="14">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001353750012640376</v>
+        <v>0.0001261659999727271</v>
       </c>
     </row>
     <row r="3">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.0009342499979538843</v>
+        <v>0.0009043329991982318</v>
       </c>
     </row>
     <row r="4">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.0002485410041117575</v>
+        <v>0.0002000829990720376</v>
       </c>
     </row>
     <row r="11">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0008862069989845622</v>
+        <v>0.0009435840038349852</v>
       </c>
     </row>
     <row r="12">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2.574538015323924e-05</v>
+        <v>2.341655985219404e-05</v>
       </c>
     </row>
     <row r="13">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1.349297006527195e-05</v>
+        <v>2.626132969453465e-05</v>
       </c>
     </row>
     <row r="14">
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001340829985565506</v>
+        <v>0.0001327089994447306</v>
       </c>
     </row>
     <row r="3">
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.002364125000895001</v>
+        <v>0.001925874996231869</v>
       </c>
     </row>
     <row r="4">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.945800174027681e-05</v>
+        <v>4.86249991809018e-05</v>
       </c>
     </row>
     <row r="11">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.002018958002736326</v>
+        <v>0.001665415999013931</v>
       </c>
     </row>
     <row r="12">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.003498007900052471</v>
+        <v>0.00138657673043781</v>
       </c>
     </row>
     <row r="13">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>6.50303599104518e-05</v>
+        <v>5.227247966104187e-05</v>
       </c>
     </row>
     <row r="14">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0001991669996641576</v>
+        <v>0.0001448749972041696</v>
       </c>
     </row>
     <row r="3">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>7.337499846471474e-05</v>
+        <v>6.858299457235262e-05</v>
       </c>
     </row>
     <row r="4">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.312499731895514e-05</v>
+        <v>4.433400317793712e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>5.63749999855645e-05</v>
+        <v>5.737499304814264e-05</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>5.652378982631489e-05</v>
+        <v>3.181365951604676e-05</v>
       </c>
     </row>
     <row r="13">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>3.881909018673468e-05</v>
+        <v>2.071372997306753e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.0002321669999219012</v>
+        <v>0.0001503750027040951</v>
       </c>
     </row>
     <row r="3">
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.00022641699979431</v>
+        <v>0.0002157080016331747</v>
       </c>
     </row>
     <row r="4">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.275000173947774e-05</v>
+        <v>4.433399590197951e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0001147090006270446</v>
+        <v>0.0001150000025518239</v>
       </c>
     </row>
     <row r="12">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.0003925650500241318</v>
+        <v>0.0001016533102665562</v>
       </c>
     </row>
     <row r="13">
@@ -1565,7 +1565,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>6.946291970962193e-05</v>
+        <v>3.18957998388214e-05</v>
       </c>
     </row>
     <row r="14">

</xml_diff>